<commit_message>
Changed how level X Card dependency is handled.
</commit_message>
<xml_diff>
--- a/sheet/SkillCardData.xlsx
+++ b/sheet/SkillCardData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspace\nanDeck\DungeonCrawlDeckMaster\sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C66EE92A-FC69-4D85-BB58-C57E998A8D83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0132A099-FE9B-4850-8E93-3198D4D0DA23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6285" yWindow="4140" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -165,19 +165,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>需要拥有《等级2》才能购买。&lt;br&gt;
-可以使用至多包含3张牌的堆叠。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>需要拥有《等级3》才能购买。&lt;br&gt;可以使用至多包含4张牌的堆叠。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>需要拥有《等级4》才能购买。&lt;br&gt;可以使用至多包含5张牌的堆叠。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>每拥有1张《手牌基数》，本牌的点数加2。&lt;br&gt;
 手牌基数加1。</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -242,6 +229,19 @@
   <si>
     <t>每拥有1张《感知》，本牌点数减1，最低为2。&lt;br&gt;
 横置本牌，将墓地顶端1张牌加入手牌。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>进入备选升级牌区时：如果玩家未拥有《等级2》，则重抽本牌。&lt;br&gt;
+可以使用至多包含3张牌的堆叠。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>进入备选升级牌区时：如果玩家未拥有《等级3》，则重抽本牌。&lt;br&gt;可以使用至多包含4张牌的堆叠。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>进入备选升级牌区时：如果玩家未拥有《等级4》，则重抽本牌。&lt;br&gt;可以使用至多包含5张牌的堆叠。</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -585,8 +585,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -625,7 +625,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="114" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" ht="171" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -633,10 +633,10 @@
         <v>3</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="114" x14ac:dyDescent="0.2">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="171" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -644,10 +644,10 @@
         <v>4</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="114" x14ac:dyDescent="0.2">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="171" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -655,7 +655,7 @@
         <v>5</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>28</v>
+        <v>42</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="114" x14ac:dyDescent="0.2">
@@ -666,12 +666,12 @@
         <v>4</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="142.5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B7">
         <v>4</v>
@@ -680,7 +680,7 @@
         <v>11</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="156.75" x14ac:dyDescent="0.2">
@@ -694,7 +694,7 @@
         <v>11</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="156.75" x14ac:dyDescent="0.2">
@@ -708,7 +708,7 @@
         <v>11</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="213.75" x14ac:dyDescent="0.2">
@@ -722,12 +722,12 @@
         <v>13</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="156.75" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B11">
         <v>5</v>
@@ -736,7 +736,7 @@
         <v>13</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="171" x14ac:dyDescent="0.2">
@@ -750,7 +750,7 @@
         <v>15</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="171" x14ac:dyDescent="0.2">
@@ -764,7 +764,7 @@
         <v>15</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="185.25" x14ac:dyDescent="0.2">
@@ -778,7 +778,7 @@
         <v>18</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="213.75" x14ac:dyDescent="0.2">
@@ -792,12 +792,12 @@
         <v>20</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="256.5" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B16">
         <v>4</v>
@@ -806,7 +806,7 @@
         <v>20</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="E16" t="e" cm="1">
         <f t="array" ref="E16">_xlfn.SWITCH(#REF!, "药水", "Potion", "食物", "Food", "弹药", "Ammo", "卷轴", "Scroll", "")</f>

</xml_diff>